<commit_message>
ùltimos cambios no añadidos
</commit_message>
<xml_diff>
--- a/client/descargas/calculadora/Modelo_CEI_DOTv2.xlsx
+++ b/client/descargas/calculadora/Modelo_CEI_DOTv2.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sayel Cortes\Dropbox\MLED\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leticia Ramos\Desktop\cts\MLED\propuesta 2015\documentos finales\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="15360" windowHeight="7155" tabRatio="789" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="15360" windowHeight="7155" tabRatio="789"/>
   </bookViews>
   <sheets>
     <sheet name="Portada" sheetId="5" r:id="rId1"/>
@@ -1169,7 +1169,7 @@
     <t>Nota: Se recomienda considerar los principales tipos de vehículos que pueden ser afectados en la implementación de un DOT, en general estos son los más comunes.</t>
   </si>
   <si>
-    <t>Pasajeros recorridos por día</t>
+    <t>Pasajeros transportados por día</t>
   </si>
 </sst>
 </file>
@@ -3373,10 +3373,10 @@
     </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
+    <cellStyle name="Hipervínculo" xfId="3" builtinId="8"/>
+    <cellStyle name="Millares" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="2" builtinId="5"/>
+    <cellStyle name="Porcentaje" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3399,7 +3399,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3475,7 +3475,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3537,7 +3537,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="es-ES"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -3648,7 +3648,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="es-ES"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -3789,7 +3789,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2120678560"/>
@@ -3831,7 +3831,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -3861,7 +3861,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-ES"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3875,7 +3875,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3946,7 +3946,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -4209,7 +4209,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="es-ES"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -4370,7 +4370,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="es-ES"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -4532,7 +4532,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2117305360"/>
@@ -4591,7 +4591,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2117308704"/>
@@ -4633,7 +4633,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -4663,7 +4663,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-ES"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4677,7 +4677,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -4747,7 +4747,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -4957,7 +4957,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2117273216"/>
@@ -5016,7 +5016,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2117276560"/>
@@ -5058,7 +5058,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -5088,7 +5088,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-ES"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -5102,7 +5102,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -5186,7 +5186,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -5534,7 +5534,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2120769152"/>
@@ -5593,7 +5593,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2120765824"/>
@@ -5635,7 +5635,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -5665,7 +5665,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-ES"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -5679,7 +5679,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -5763,7 +5763,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -6121,7 +6121,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2117214944"/>
@@ -6180,7 +6180,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2117218288"/>
@@ -6232,7 +6232,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -6262,7 +6262,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-ES"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -6276,7 +6276,7 @@
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -6339,7 +6339,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -6413,7 +6413,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="es-ES"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -6524,7 +6524,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="es-ES"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -6665,7 +6665,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2119694080"/>
@@ -6708,7 +6708,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-ES"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -6738,7 +6738,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-ES"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -10680,11 +10680,11 @@
   </sheetPr>
   <dimension ref="B5:K37"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="89" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="89" workbookViewId="0">
       <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="1.7109375" customWidth="1"/>
     <col min="3" max="3" width="19.42578125" customWidth="1"/>
@@ -11069,12 +11069,12 @@
   </sheetPr>
   <dimension ref="B1:N62"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B1" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N27" sqref="N27:N28"/>
+    <sheetView showGridLines="0" zoomScale="73" zoomScaleNormal="73" zoomScalePageLayoutView="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="1.7109375" customWidth="1"/>
     <col min="2" max="2" width="46.5703125" customWidth="1"/>
@@ -11089,7 +11089,7 @@
     <col min="11" max="11" width="7.28515625" customWidth="1"/>
     <col min="12" max="12" width="16" customWidth="1"/>
     <col min="13" max="13" width="19" customWidth="1"/>
-    <col min="14" max="14" width="13.42578125" customWidth="1"/>
+    <col min="14" max="14" width="14.5703125" customWidth="1"/>
     <col min="15" max="15" width="14.42578125" customWidth="1"/>
     <col min="19" max="19" width="4.140625" customWidth="1"/>
   </cols>
@@ -11533,7 +11533,7 @@
         <v>130</v>
       </c>
       <c r="D26" s="189"/>
-      <c r="E26" s="189"/>
+      <c r="E26" s="190"/>
       <c r="F26" s="37">
         <v>1.2</v>
       </c>
@@ -12333,7 +12333,7 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="1.42578125" customWidth="1"/>
     <col min="2" max="2" width="36" style="223" customWidth="1"/>
@@ -13874,11 +13874,11 @@
   <dimension ref="B1:R39"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="1.7109375" customWidth="1"/>
     <col min="2" max="2" width="47.28515625" bestFit="1" customWidth="1"/>
@@ -15018,12 +15018,12 @@
   </sheetPr>
   <dimension ref="B1:T73"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="J51" sqref="J51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="1.42578125" customWidth="1"/>
     <col min="2" max="2" width="57.42578125" customWidth="1"/>
@@ -16988,7 +16988,7 @@
       <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="1.7109375" customWidth="1"/>
     <col min="2" max="2" width="8.42578125" customWidth="1"/>
@@ -18262,7 +18262,7 @@
       <selection pane="bottomLeft" activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="1.42578125" customWidth="1"/>
     <col min="2" max="2" width="59" bestFit="1" customWidth="1"/>
@@ -19569,7 +19569,7 @@
       <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="1.7109375" customWidth="1"/>
     <col min="2" max="2" width="38.28515625" customWidth="1"/>

</xml_diff>